<commit_message>
DDT using excel for multi data using for ,added new col , set data in the col,exceloprtaionclass
</commit_message>
<xml_diff>
--- a/src/test/java/com/TestData/ExcelFacebookReg/FacebookReg.xlsx
+++ b/src/test/java/com/TestData/ExcelFacebookReg/FacebookReg.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\VWOLoginAutomationSeleniumTestNG\src\test\java\com\TestDataFacebookReg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\DataDrivenTesting\src\test\java\com\TestData\ExcelFacebookReg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7833366-639D-4F9C-AD49-C399145A3DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F62FF9-52EC-4474-93AA-08BAEAD741AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C9F0C498-F276-42DE-A6D2-BDB82F9DA260}"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
+    <sheet name="satyam" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>mobile</t>
   </si>
@@ -74,12 +75,34 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>satyam</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Q@123</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>newdata</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,9 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,19 +460,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA3158D-4030-4AD3-A698-CEF7900D8C8C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="5.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -459,47 +484,91 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>9022341891</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>7485749382</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>9273645183</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3425252625</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -510,12 +579,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.9453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.9453125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="7.9453125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>